<commit_message>
added data with 1000uL tip
</commit_message>
<xml_diff>
--- a/data/commerical-Vs-printed-comparison/data-taking-raw/printed-pipette-3mL-syringe-100uL-160217.xlsx
+++ b/data/commerical-Vs-printed-comparison/data-taking-raw/printed-pipette-3mL-syringe-100uL-160217.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="8">
   <si>
     <t>Trial 1</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>200uL Tip</t>
+  </si>
+  <si>
+    <t>1000uL Tip</t>
   </si>
 </sst>
 </file>
@@ -362,10 +365,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -381,127 +384,258 @@
         <v>6</v>
       </c>
     </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>101.4</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>100</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>102.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>101.1</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>99</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>102.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>100.9</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>99.5</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5">
+        <v>103.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>101.1</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>99.5</v>
+      </c>
+      <c r="G6">
+        <v>4</v>
+      </c>
+      <c r="H6">
+        <v>102.7</v>
+      </c>
+    </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>102.3</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>98.6</v>
+      </c>
+      <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="H7">
+        <v>102.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>0</v>
       </c>
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
-        <v>3</v>
-      </c>
-      <c r="G7" t="s">
-        <v>2</v>
-      </c>
-      <c r="H7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8">
-        <v>101.4</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>100</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-      <c r="H8">
-        <v>102.2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>2</v>
-      </c>
-      <c r="B9">
-        <v>101.1</v>
-      </c>
-      <c r="D9">
-        <v>2</v>
-      </c>
-      <c r="E9">
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>93</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>85.6</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>97.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>88.1</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>89.9</v>
+      </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
+      <c r="H14">
+        <v>98.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>3</v>
+      </c>
+      <c r="B15">
+        <v>92.6</v>
+      </c>
+      <c r="D15">
+        <v>3</v>
+      </c>
+      <c r="E15">
+        <v>91.7</v>
+      </c>
+      <c r="G15">
+        <v>3</v>
+      </c>
+      <c r="H15">
         <v>99</v>
       </c>
-      <c r="G9">
-        <v>2</v>
-      </c>
-      <c r="H9">
-        <v>102.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>3</v>
-      </c>
-      <c r="B10">
-        <v>100.9</v>
-      </c>
-      <c r="D10">
-        <v>3</v>
-      </c>
-      <c r="E10">
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16">
+        <v>93.7</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+      <c r="E16">
+        <v>91.1</v>
+      </c>
+      <c r="G16">
+        <v>4</v>
+      </c>
+      <c r="H16">
         <v>99.5</v>
       </c>
-      <c r="G10">
-        <v>3</v>
-      </c>
-      <c r="H10">
-        <v>103.6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>4</v>
-      </c>
-      <c r="B11">
-        <v>101.1</v>
-      </c>
-      <c r="D11">
-        <v>4</v>
-      </c>
-      <c r="E11">
-        <v>99.5</v>
-      </c>
-      <c r="G11">
-        <v>4</v>
-      </c>
-      <c r="H11">
-        <v>102.7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>5</v>
-      </c>
-      <c r="B12">
-        <v>102.3</v>
-      </c>
-      <c r="D12">
-        <v>5</v>
-      </c>
-      <c r="E12">
-        <v>98.6</v>
-      </c>
-      <c r="G12">
-        <v>5</v>
-      </c>
-      <c r="H12">
-        <v>102.4</v>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>5</v>
+      </c>
+      <c r="B17">
+        <v>92.2</v>
+      </c>
+      <c r="D17">
+        <v>5</v>
+      </c>
+      <c r="E17">
+        <v>91.6</v>
+      </c>
+      <c r="G17">
+        <v>5</v>
+      </c>
+      <c r="H17">
+        <v>100.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>